<commit_message>
Day 8 Commit before delete
</commit_message>
<xml_diff>
--- a/arun_day7_error-and-solutions .xlsx
+++ b/arun_day7_error-and-solutions .xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
   <si>
     <t>S.No</t>
   </si>
@@ -185,6 +185,9 @@
   </si>
   <si>
     <t>Image uploading using MultiPart</t>
+  </si>
+  <si>
+    <t>http://www.journaldev.com/2573/spring-mvc-file-upload-example-single-multiple-files      http://www.devmanuals.com/tutorials/java/spring/spring3/mvc/spring3-mvc-upload-file.html</t>
   </si>
 </sst>
 </file>
@@ -621,7 +624,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -632,7 +635,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -673,7 +676,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" ht="45">
       <c r="A2" s="18">
         <v>1</v>
       </c>
@@ -684,12 +687,12 @@
         <v>45</v>
       </c>
       <c r="D2" s="14"/>
-      <c r="E2" s="9"/>
+      <c r="E2" s="9" t="s">
+        <v>46</v>
+      </c>
       <c r="F2" s="14"/>
       <c r="G2" s="18"/>
-      <c r="H2" s="18">
-        <v>7</v>
-      </c>
+      <c r="H2" s="18"/>
     </row>
     <row r="3" spans="1:8" ht="45.75" customHeight="1">
       <c r="A3" s="18"/>
@@ -782,8 +785,11 @@
       <c r="H11" s="18"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" display="http://www.journaldev.com/2573/spring-mvc-file-upload-example-single-multiple-files"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>